<commit_message>
Updated Serial and Parallel Comparison
Updated the parallel times for the serial vs parallel comparison so
that it would a fair comparison between the two with no early stopping
for each.
</commit_message>
<xml_diff>
--- a/Weak and Strong Scaling.xlsx
+++ b/Weak and Strong Scaling.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="20480" windowHeight="25060" tabRatio="500"/>
+    <workbookView xWindow="17620" yWindow="1020" windowWidth="20480" windowHeight="25060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>Threads</t>
   </si>
@@ -66,14 +66,24 @@
   </si>
   <si>
     <t>Number of elements</t>
+  </si>
+  <si>
+    <t>Early Stopping</t>
+  </si>
+  <si>
+    <t>No early stopping</t>
+  </si>
+  <si>
+    <t>No Early Stopping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -129,7 +139,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -210,18 +220,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -261,6 +274,7 @@
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -300,6 +314,7 @@
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -576,15 +591,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3:U6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -597,11 +612,23 @@
       <c r="N1" t="s">
         <v>11</v>
       </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
       <c r="S1" t="s">
         <v>12</v>
       </c>
+      <c r="T1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -650,8 +677,20 @@
       <c r="V2" t="s">
         <v>13</v>
       </c>
+      <c r="X2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -685,7 +724,7 @@
       <c r="O3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="6">
         <v>0.20857999999999999</v>
       </c>
       <c r="Q3">
@@ -698,15 +737,28 @@
       <c r="T3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="6">
         <v>27.778331000000001</v>
       </c>
       <c r="V3">
         <f>10*15</f>
         <v>150</v>
       </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>320.83676600000001</v>
+      </c>
+      <c r="AA3">
+        <f>10*15</f>
+        <v>150</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -731,7 +783,7 @@
         <v>35.430635000000002</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" ref="K4:K7" si="1">$J$3/J4</f>
+        <f t="shared" ref="K4:K5" si="1">$J$3/J4</f>
         <v>0.78402012834373414</v>
       </c>
       <c r="N4">
@@ -740,7 +792,7 @@
       <c r="O4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="6">
         <v>0.68680699999999995</v>
       </c>
       <c r="Q4">
@@ -753,15 +805,28 @@
       <c r="T4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="6">
         <v>44.095233999999998</v>
       </c>
       <c r="V4">
         <f>20*30</f>
         <v>600</v>
       </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>650.53580799999997</v>
+      </c>
+      <c r="AA4">
+        <f>20*30</f>
+        <v>600</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -795,7 +860,7 @@
       <c r="O5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="6">
         <v>3.2735910000000001</v>
       </c>
       <c r="Q5">
@@ -808,15 +873,28 @@
       <c r="T5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="6">
         <v>125.84800199999999</v>
       </c>
       <c r="V5">
         <f>40*60</f>
         <v>2400</v>
       </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>2765.6028040000001</v>
+      </c>
+      <c r="AA5">
+        <f>40*60</f>
+        <v>2400</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>16</v>
       </c>
@@ -839,7 +917,7 @@
       <c r="O6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="6">
         <v>20.701391999999998</v>
       </c>
       <c r="Q6">
@@ -852,15 +930,28 @@
       <c r="T6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="6">
         <v>9634.5675200000005</v>
       </c>
       <c r="V6">
         <f>80*120</f>
         <v>9600</v>
       </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>9634.5675200000005</v>
+      </c>
+      <c r="AA6">
+        <f>80*120</f>
+        <v>9600</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>

</xml_diff>